<commit_message>
fixed labels to include all attendence types
</commit_message>
<xml_diff>
--- a/charts_output/charts_report.xlsx
+++ b/charts_output/charts_report.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>Name</t>
   </si>
@@ -27,33 +27,6 @@
     <t>Jan Kowalski</t>
   </si>
   <si>
-    <t>Jan2 Kowalski</t>
-  </si>
-  <si>
-    <t>Jan3 Kowalski</t>
-  </si>
-  <si>
-    <t>Jan4 Kowalski</t>
-  </si>
-  <si>
-    <t>Jan5 Kowalski</t>
-  </si>
-  <si>
-    <t>Michal Kowalski</t>
-  </si>
-  <si>
-    <t>Michal2 Kowalski</t>
-  </si>
-  <si>
-    <t>Michal3 Kowalski</t>
-  </si>
-  <si>
-    <t>Michal4 Kowalski</t>
-  </si>
-  <si>
-    <t>Michal5 Kowalski</t>
-  </si>
-  <si>
     <t>Student</t>
   </si>
   <si>
@@ -64,6 +37,9 @@
   </si>
   <si>
     <t>NOTPRESENT</t>
+  </si>
+  <si>
+    <t>JUSTIFIED</t>
   </si>
   <si>
     <t>Date</t>
@@ -560,7 +536,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A16:B26"/>
+  <dimension ref="A16:B17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -582,78 +558,6 @@
         <v>4.428571428571429</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
-      <c r="A18" t="s">
-        <v>3</v>
-      </c>
-      <c r="B18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2">
-      <c r="A19" t="s">
-        <v>4</v>
-      </c>
-      <c r="B19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2">
-      <c r="A20" t="s">
-        <v>5</v>
-      </c>
-      <c r="B20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2">
-      <c r="A21" t="s">
-        <v>6</v>
-      </c>
-      <c r="B21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2">
-      <c r="A22" t="s">
-        <v>7</v>
-      </c>
-      <c r="B22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2">
-      <c r="A23" t="s">
-        <v>8</v>
-      </c>
-      <c r="B23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2">
-      <c r="A24" t="s">
-        <v>9</v>
-      </c>
-      <c r="B24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2">
-      <c r="A25" t="s">
-        <v>10</v>
-      </c>
-      <c r="B25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2">
-      <c r="A26" t="s">
-        <v>11</v>
-      </c>
-      <c r="B26">
-        <v>0</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -662,27 +566,30 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A16:D26"/>
+  <dimension ref="A16:E17"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:5">
       <c r="A16" s="1" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
+        <v>6</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
       <c r="A17" t="s">
         <v>2</v>
       </c>
@@ -695,130 +602,7 @@
       <c r="D17">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="A18" t="s">
-        <v>3</v>
-      </c>
-      <c r="B18">
-        <v>0</v>
-      </c>
-      <c r="C18">
-        <v>0</v>
-      </c>
-      <c r="D18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
-      <c r="A19" t="s">
-        <v>4</v>
-      </c>
-      <c r="B19">
-        <v>0</v>
-      </c>
-      <c r="C19">
-        <v>0</v>
-      </c>
-      <c r="D19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
-      <c r="A20" t="s">
-        <v>5</v>
-      </c>
-      <c r="B20">
-        <v>0</v>
-      </c>
-      <c r="C20">
-        <v>0</v>
-      </c>
-      <c r="D20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4">
-      <c r="A21" t="s">
-        <v>6</v>
-      </c>
-      <c r="B21">
-        <v>0</v>
-      </c>
-      <c r="C21">
-        <v>0</v>
-      </c>
-      <c r="D21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4">
-      <c r="A22" t="s">
-        <v>7</v>
-      </c>
-      <c r="B22">
-        <v>0</v>
-      </c>
-      <c r="C22">
-        <v>0</v>
-      </c>
-      <c r="D22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4">
-      <c r="A23" t="s">
-        <v>8</v>
-      </c>
-      <c r="B23">
-        <v>0</v>
-      </c>
-      <c r="C23">
-        <v>0</v>
-      </c>
-      <c r="D23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4">
-      <c r="A24" t="s">
-        <v>9</v>
-      </c>
-      <c r="B24">
-        <v>0</v>
-      </c>
-      <c r="C24">
-        <v>0</v>
-      </c>
-      <c r="D24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4">
-      <c r="A25" t="s">
-        <v>10</v>
-      </c>
-      <c r="B25">
-        <v>0</v>
-      </c>
-      <c r="C25">
-        <v>0</v>
-      </c>
-      <c r="D25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4">
-      <c r="A26" t="s">
-        <v>11</v>
-      </c>
-      <c r="B26">
-        <v>0</v>
-      </c>
-      <c r="C26">
-        <v>0</v>
-      </c>
-      <c r="D26">
+      <c r="E17">
         <v>0</v>
       </c>
     </row>
@@ -838,10 +622,10 @@
   <sheetData>
     <row r="16" spans="1:2">
       <c r="A16" s="1" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
     <row r="17" spans="1:2">

</xml_diff>